<commit_message>
Did a lot of work, and good progress on emails
</commit_message>
<xml_diff>
--- a/uploads/students.xlsx
+++ b/uploads/students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Student Registration Number</t>
   </si>
@@ -30,36 +30,18 @@
     <t>Parent 1 Name</t>
   </si>
   <si>
-    <t>Parent 1 Email 1</t>
-  </si>
-  <si>
-    <t>Parent 1 Email 2</t>
-  </si>
-  <si>
     <t>Parent 1 Phone Numbers</t>
   </si>
   <si>
     <t>Parent 2 Name</t>
   </si>
   <si>
-    <t>Parent 2 Email 1</t>
-  </si>
-  <si>
-    <t>Parent 2 Email 2</t>
-  </si>
-  <si>
     <t>Parent 2 Phone Numbers</t>
   </si>
   <si>
     <t>Parent 3 Name</t>
   </si>
   <si>
-    <t>Parent 3 Email 1</t>
-  </si>
-  <si>
-    <t>Parent 3 Email 2</t>
-  </si>
-  <si>
     <t>Parent 3 Phone Numbers</t>
   </si>
   <si>
@@ -75,22 +57,25 @@
     <t>mwenda.lilian@yahoo.com</t>
   </si>
   <si>
-    <t>lilian.mwenda@gmail.com</t>
-  </si>
-  <si>
     <t>Thomas Silonad</t>
   </si>
   <si>
     <t>Vusimuzi@gmail.com</t>
   </si>
   <si>
-    <t>silonda@gmail.com</t>
-  </si>
-  <si>
     <t>Deborah Mwenda</t>
   </si>
   <si>
     <t>info@bahari.org</t>
+  </si>
+  <si>
+    <t>Parent 1 Email</t>
+  </si>
+  <si>
+    <t>Parent 2 Email</t>
+  </si>
+  <si>
+    <t>Parent 3 Email</t>
   </si>
 </sst>
 </file>
@@ -440,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,15 +438,16 @@
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,97 +461,82 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100101</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="F2">
         <v>784540459</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100101</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>784540459</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3">
-        <v>784540459</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3">
+      <c r="L3">
         <v>713617634</v>
       </c>
     </row>
@@ -573,10 +544,8 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="I3" r:id="rId4"/>
-    <hyperlink ref="J3" r:id="rId5"/>
-    <hyperlink ref="M3" r:id="rId6"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="K3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>